<commit_message>
Tweak to Panth2013 data
</commit_message>
<xml_diff>
--- a/data/panth2013_case_data.xlsx
+++ b/data/panth2013_case_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5568"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5565"/>
   </bookViews>
   <sheets>
     <sheet name="Design Data" sheetId="2" r:id="rId1"/>
@@ -441,15 +441,15 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
@@ -469,7 +469,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -489,7 +489,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>16</v>
       </c>
@@ -510,7 +510,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>17</v>
       </c>
@@ -532,7 +532,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>18</v>
       </c>
@@ -553,75 +553,75 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:17" x14ac:dyDescent="0.25">
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="22" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -629,7 +629,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -637,7 +637,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -646,7 +646,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:17" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -655,7 +655,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -664,7 +664,7 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="7:17" x14ac:dyDescent="0.25">
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -672,7 +672,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="7:17" x14ac:dyDescent="0.25">
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -680,7 +680,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="7:17" x14ac:dyDescent="0.25">
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -688,7 +688,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:17" x14ac:dyDescent="0.25">
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -696,7 +696,7 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:17" x14ac:dyDescent="0.25">
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -704,13 +704,13 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="7:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="7:17" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="G35" s="1"/>
@@ -720,7 +720,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -729,7 +729,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -738,7 +738,7 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -747,7 +747,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -756,7 +756,7 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -764,7 +764,7 @@
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -772,7 +772,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -780,7 +780,7 @@
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -788,7 +788,7 @@
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -796,7 +796,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -804,7 +804,7 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="48" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="G48" s="1"/>
@@ -812,7 +812,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="G49" s="1"/>
@@ -820,7 +820,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -829,7 +829,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -838,7 +838,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -847,7 +847,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -856,7 +856,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -865,7 +865,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -874,7 +874,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -883,7 +883,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:13" x14ac:dyDescent="0.25">
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -891,7 +891,7 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -908,31 +908,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
@@ -970,7 +971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1010,7 @@
         <v>11.24</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>11.86</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>2</v>
       </c>
@@ -1081,7 +1082,7 @@
         <v>8.5500000000000007</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>3</v>
       </c>
@@ -1117,7 +1118,7 @@
         <v>7.29</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>4</v>
       </c>
@@ -1153,7 +1154,7 @@
         <v>6.41</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>2</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>21.16</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>3</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>30.26</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>4</v>
       </c>
@@ -1261,7 +1262,7 @@
         <v>48.12</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>2</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>12.71</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>3</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>11.72</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>4</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>7.29</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1446,7 +1447,7 @@
         <v>4.71</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
@@ -1482,7 +1483,7 @@
         <v>4.7300000000000004</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>2</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>3</v>
       </c>
@@ -1554,7 +1555,7 @@
         <v>3.61</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>4</v>
       </c>
@@ -1590,7 +1591,7 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>2</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>7.49</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>3</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>11.51</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>4</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>2</v>
       </c>
@@ -1734,7 +1735,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>3</v>
       </c>
@@ -1770,7 +1771,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>4</v>
       </c>
@@ -1806,7 +1807,7 @@
         <v>3.45</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>15</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>17</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>1</v>
       </c>
@@ -1919,7 +1920,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>2</v>
       </c>
@@ -1955,7 +1956,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>3</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>5.0599999999999996</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>4</v>
       </c>
@@ -2027,7 +2028,7 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>2</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>9.2200000000000006</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>3</v>
       </c>
@@ -2099,7 +2100,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>4</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>16.670000000000002</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>2</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>6.82</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>3</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>6.24</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>4</v>
       </c>
@@ -2243,10 +2244,10 @@
         <v>5.74</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>15</v>
       </c>
@@ -2284,7 +2285,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>18</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>144.41</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>1</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>206.1</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>2</v>
       </c>
@@ -2395,7 +2396,7 @@
         <v>146.5</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>3</v>
       </c>
@@ -2431,7 +2432,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>4</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>111.2</v>
       </c>
     </row>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>2</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>304.39999999999998</v>
       </c>
     </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>3</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>373.1</v>
       </c>
     </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>4</v>
       </c>
@@ -2575,7 +2576,7 @@
         <v>376.5</v>
       </c>
     </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>2</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>187.4</v>
       </c>
     </row>
-    <row r="54" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>3</v>
       </c>
@@ -2647,7 +2648,7 @@
         <v>180.2</v>
       </c>
     </row>
-    <row r="55" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>4</v>
       </c>

</xml_diff>